<commit_message>
Updated PCBWay entry with latest info
</commit_message>
<xml_diff>
--- a/Sponsors_tracker.xlsx
+++ b/Sponsors_tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxime\Desktop\Projet Perso\C3I\Github\Fork\documents_sponsors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neiz2\Documents\GitHub\documents_sponsors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59369859-E3A4-44C0-848D-6D27FAA85ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0190EEF9-4649-4D10-A1C5-CBAB414562B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="110">
   <si>
     <t>Nom de la compagnie:</t>
   </si>
@@ -360,6 +360,12 @@
   </si>
   <si>
     <t>Maxime Leblanc</t>
+  </si>
+  <si>
+    <t>sponsor@PCBWay.com</t>
+  </si>
+  <si>
+    <t>Samuel S.</t>
   </si>
 </sst>
 </file>
@@ -424,13 +430,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -794,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1008,7 @@
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1196,11 +1201,14 @@
       <c r="B20" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="D20" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="F20" t="s">
-        <v>14</v>
+        <v>109</v>
       </c>
       <c r="G20" s="4">
-        <v>45945</v>
+        <v>46063</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1317,7 +1325,7 @@
       <c r="A28" t="s">
         <v>101</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="1" t="s">
         <v>102</v>
       </c>
       <c r="E28" t="s">
@@ -1331,7 +1339,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>105</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1387,35 +1395,16 @@
     <hyperlink ref="D21" r:id="rId39" xr:uid="{89156B4A-71FB-4F13-9FBB-24BC0399790D}"/>
     <hyperlink ref="B28" r:id="rId40" xr:uid="{F3B1B291-4F14-462E-8A9D-E98522D69A4D}"/>
     <hyperlink ref="B29" r:id="rId41" xr:uid="{37FEE954-3E44-4D72-9603-F876246EB356}"/>
+    <hyperlink ref="D20" r:id="rId42" xr:uid="{D5854C0B-E945-4057-9694-433BCC876EAF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId42"/>
+    <tablePart r:id="rId43"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="05dc0aba-4466-4464-ae54-e30ec1d1960e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3ab60a15-fb7d-489d-9e0d-4f2626c05be0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100873BCB8DB02F314E9B33D47D2328BEE3" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="e554ae5040b51359eb2ce52773233a0a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3ab60a15-fb7d-489d-9e0d-4f2626c05be0" xmlns:ns3="05dc0aba-4466-4464-ae54-e30ec1d1960e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19c39bb3469a366f9905408a925319f0" ns2:_="" ns3:_="">
     <xsd:import namespace="3ab60a15-fb7d-489d-9e0d-4f2626c05be0"/>
@@ -1610,26 +1599,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A185DED4-5536-4DE8-9ED1-973A2272A88F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="05dc0aba-4466-4464-ae54-e30ec1d1960e"/>
-    <ds:schemaRef ds:uri="3ab60a15-fb7d-489d-9e0d-4f2626c05be0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E9BF95E-040F-4DB3-8CBA-B5E6AB45C8E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="05dc0aba-4466-4464-ae54-e30ec1d1960e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3ab60a15-fb7d-489d-9e0d-4f2626c05be0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9257EC00-C374-4722-9DA7-ED3C4D9C653E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1646,4 +1636,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E9BF95E-040F-4DB3-8CBA-B5E6AB45C8E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A185DED4-5536-4DE8-9ED1-973A2272A88F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="05dc0aba-4466-4464-ae54-e30ec1d1960e"/>
+    <ds:schemaRef ds:uri="3ab60a15-fb7d-489d-9e0d-4f2626c05be0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>